<commit_message>
Minor changes to reflect_loss_beckmann.  Tests now pass.
Resolves Issue #64 and #65.
</commit_message>
<xml_diff>
--- a/ocean/test/reflect_loss_beckmann_test.xlsx
+++ b/ocean/test/reflect_loss_beckmann_test.xlsx
@@ -1142,31 +1142,31 @@
                   <c:v>20.4786</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>21.4998</c:v>
+                  <c:v>21.3843</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>22.658000000000001</c:v>
+                  <c:v>21.3843</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>23.9953</c:v>
+                  <c:v>21.3843</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>25.577400000000001</c:v>
+                  <c:v>21.3843</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>27.513999999999999</c:v>
+                  <c:v>21.3843</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>30.0106</c:v>
+                  <c:v>21.3843</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>33.528199999999998</c:v>
+                  <c:v>21.3843</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>39.5306</c:v>
+                  <c:v>21.3843</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>62.835700000000003</c:v>
+                  <c:v>21.3843</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1725,31 +1725,31 @@
                   <c:v>21.962700000000002</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>22.983899999999998</c:v>
+                  <c:v>22.868400000000001</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>24.141999999999999</c:v>
+                  <c:v>22.868400000000001</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>25.479399999999998</c:v>
+                  <c:v>22.868400000000001</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>27.061399999999999</c:v>
+                  <c:v>22.868400000000001</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>28.998000000000001</c:v>
+                  <c:v>22.868400000000001</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>31.494700000000002</c:v>
+                  <c:v>22.868400000000001</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>35.012300000000003</c:v>
+                  <c:v>22.868400000000001</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>41.014600000000002</c:v>
+                  <c:v>22.868400000000001</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>64.319800000000001</c:v>
+                  <c:v>22.868400000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2314,25 +2314,25 @@
                   <c:v>25.184999999999999</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>26.128799999999998</c:v>
+                  <c:v>26.098500000000001</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>27.146000000000001</c:v>
+                  <c:v>26.098500000000001</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>28.232099999999999</c:v>
+                  <c:v>26.098500000000001</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>29.364899999999999</c:v>
+                  <c:v>26.098500000000001</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>30.486599999999999</c:v>
+                  <c:v>26.098500000000001</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>31.4773</c:v>
+                  <c:v>26.098500000000001</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>32.146900000000002</c:v>
+                  <c:v>26.098500000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2897,25 +2897,25 @@
                   <c:v>29.24</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>30.183800000000002</c:v>
+                  <c:v>30.153500000000001</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>31.201000000000001</c:v>
+                  <c:v>30.153500000000001</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>32.287100000000002</c:v>
+                  <c:v>30.153500000000001</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>33.419899999999998</c:v>
+                  <c:v>30.153500000000001</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>34.541600000000003</c:v>
+                  <c:v>30.153500000000001</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>35.532400000000003</c:v>
+                  <c:v>30.153500000000001</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>36.201900000000002</c:v>
+                  <c:v>30.153500000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2930,11 +2930,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="53389568"/>
-        <c:axId val="53388032"/>
+        <c:axId val="115758592"/>
+        <c:axId val="115760512"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="53389568"/>
+        <c:axId val="115758592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10"/>
@@ -2977,12 +2977,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53388032"/>
+        <c:crossAx val="115760512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="53388032"/>
+        <c:axId val="115760512"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="12"/>
@@ -3025,7 +3025,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53389568"/>
+        <c:crossAx val="115758592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3052,15 +3052,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>19049</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:colOff>295274</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>561974</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>228599</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3372,7 +3372,7 @@
   <dimension ref="A1:E92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4793,10 +4793,10 @@
         <v>82</v>
       </c>
       <c r="B84">
-        <v>21.4998</v>
+        <v>21.3843</v>
       </c>
       <c r="C84">
-        <v>22.983899999999998</v>
+        <v>22.868400000000001</v>
       </c>
       <c r="D84">
         <v>24.311499999999999</v>
@@ -4810,10 +4810,10 @@
         <v>83</v>
       </c>
       <c r="B85">
-        <v>22.658000000000001</v>
+        <v>21.3843</v>
       </c>
       <c r="C85">
-        <v>24.141999999999999</v>
+        <v>22.868400000000001</v>
       </c>
       <c r="D85">
         <v>25.184999999999999</v>
@@ -4827,16 +4827,16 @@
         <v>84</v>
       </c>
       <c r="B86">
-        <v>23.9953</v>
+        <v>21.3843</v>
       </c>
       <c r="C86">
-        <v>25.479399999999998</v>
+        <v>22.868400000000001</v>
       </c>
       <c r="D86">
-        <v>26.128799999999998</v>
+        <v>26.098500000000001</v>
       </c>
       <c r="E86">
-        <v>30.183800000000002</v>
+        <v>30.153500000000001</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -4844,16 +4844,16 @@
         <v>85</v>
       </c>
       <c r="B87">
-        <v>25.577400000000001</v>
+        <v>21.3843</v>
       </c>
       <c r="C87">
-        <v>27.061399999999999</v>
+        <v>22.868400000000001</v>
       </c>
       <c r="D87">
-        <v>27.146000000000001</v>
+        <v>26.098500000000001</v>
       </c>
       <c r="E87">
-        <v>31.201000000000001</v>
+        <v>30.153500000000001</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -4861,16 +4861,16 @@
         <v>86</v>
       </c>
       <c r="B88">
-        <v>27.513999999999999</v>
+        <v>21.3843</v>
       </c>
       <c r="C88">
-        <v>28.998000000000001</v>
+        <v>22.868400000000001</v>
       </c>
       <c r="D88">
-        <v>28.232099999999999</v>
+        <v>26.098500000000001</v>
       </c>
       <c r="E88">
-        <v>32.287100000000002</v>
+        <v>30.153500000000001</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
@@ -4878,16 +4878,16 @@
         <v>87</v>
       </c>
       <c r="B89">
-        <v>30.0106</v>
+        <v>21.3843</v>
       </c>
       <c r="C89">
-        <v>31.494700000000002</v>
+        <v>22.868400000000001</v>
       </c>
       <c r="D89">
-        <v>29.364899999999999</v>
+        <v>26.098500000000001</v>
       </c>
       <c r="E89">
-        <v>33.419899999999998</v>
+        <v>30.153500000000001</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -4895,16 +4895,16 @@
         <v>88</v>
       </c>
       <c r="B90">
-        <v>33.528199999999998</v>
+        <v>21.3843</v>
       </c>
       <c r="C90">
-        <v>35.012300000000003</v>
+        <v>22.868400000000001</v>
       </c>
       <c r="D90">
-        <v>30.486599999999999</v>
+        <v>26.098500000000001</v>
       </c>
       <c r="E90">
-        <v>34.541600000000003</v>
+        <v>30.153500000000001</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -4912,16 +4912,16 @@
         <v>89</v>
       </c>
       <c r="B91">
-        <v>39.5306</v>
+        <v>21.3843</v>
       </c>
       <c r="C91">
-        <v>41.014600000000002</v>
+        <v>22.868400000000001</v>
       </c>
       <c r="D91">
-        <v>31.4773</v>
+        <v>26.098500000000001</v>
       </c>
       <c r="E91">
-        <v>35.532400000000003</v>
+        <v>30.153500000000001</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -4929,16 +4929,16 @@
         <v>90</v>
       </c>
       <c r="B92">
-        <v>62.835700000000003</v>
+        <v>21.3843</v>
       </c>
       <c r="C92">
-        <v>64.319800000000001</v>
+        <v>22.868400000000001</v>
       </c>
       <c r="D92">
-        <v>32.146900000000002</v>
+        <v>26.098500000000001</v>
       </c>
       <c r="E92">
-        <v>36.201900000000002</v>
+        <v>30.153500000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>